<commit_message>
release ITI.Scheduling 1.0.0 for TI
</commit_message>
<xml_diff>
--- a/ITI/Scheduling/CodeSystem-status-reason.xlsx
+++ b/ITI/Scheduling/CodeSystem-status-reason.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0-comment</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -270,7 +270,7 @@
     <t>Patient Needs Tests</t>
   </si>
   <si>
-    <t>An appointment for a patient was cancelled by the patient because the patient did not have the prequisite diagnostic tests performed.</t>
+    <t>An appointment for a patient was cancelled by the patient because the patient did not have the prerequisite diagnostic tests performed.</t>
   </si>
   <si>
     <t>new-provider</t>
@@ -342,7 +342,7 @@
     <t>Preparatory Requirements or Medications Incomplete</t>
   </si>
   <si>
-    <t>An appointment for a patient was cancelled by the provider because needed preparatory insructions and/or medications not completed.</t>
+    <t>An appointment for a patient was cancelled by the provider because needed preparatory instructions and/or medications not completed.</t>
   </si>
   <si>
     <t>prep-unavail</t>

</xml_diff>